<commit_message>
added 1,3 guessers to excel
</commit_message>
<xml_diff>
--- a/LLMs/Analysis_Performance.xlsx
+++ b/LLMs/Analysis_Performance.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1271,6 +1271,114 @@
         <v>0.6666666666666666</v>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>3_guesser</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>9.272727272727273</v>
+      </c>
+      <c r="C16" t="n">
+        <v>5.818181818181818</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.1818181818181818</v>
+      </c>
+      <c r="E16" t="n">
+        <v>1.363636363636364</v>
+      </c>
+      <c r="F16" t="n">
+        <v>1.363636363636364</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.1818181818181818</v>
+      </c>
+      <c r="H16" t="n">
+        <v>4.727272727272728</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.1818181818181818</v>
+      </c>
+      <c r="J16" t="n">
+        <v>1.090909090909091</v>
+      </c>
+      <c r="K16" t="n">
+        <v>1</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0.09090909090909091</v>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>RED</t>
+        </is>
+      </c>
+      <c r="N16" t="n">
+        <v>54.54545454545454</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0.6530612244897959</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>1_guesser</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>7.727272727272728</v>
+      </c>
+      <c r="C17" t="n">
+        <v>5</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.2727272727272727</v>
+      </c>
+      <c r="E17" t="n">
+        <v>1.090909090909091</v>
+      </c>
+      <c r="F17" t="n">
+        <v>1.454545454545455</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.1818181818181818</v>
+      </c>
+      <c r="H17" t="n">
+        <v>4.090909090909091</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.2727272727272727</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.6363636363636364</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.9090909090909091</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.09090909090909091</v>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>BLUE</t>
+        </is>
+      </c>
+      <c r="N17" t="n">
+        <v>54.54545454545454</v>
+      </c>
+      <c r="O17" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="P17" t="n">
+        <v>0.6818181818181818</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>